<commit_message>
Update: 1508 stocks from 80 managers [2025-06-24]
</commit_message>
<xml_diff>
--- a/analysis/dataroma_analysis.xlsx
+++ b/analysis/dataroma_analysis.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-23 16:35:03</t>
+          <t>2025-06-24 00:28:22</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.902811819595646</t>
+          <t>2.901863141524106</t>
         </is>
       </c>
     </row>
@@ -2074,15 +2074,15 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>HTZWW</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Francois Rochon - Giverny Capital, Polen Capital Management, Yacktman Asset Management</t>
+          <t>Daniel Loeb - Third Point, Francis Chou - Chou Associates</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -2090,13 +2090,13 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>28.3</v>
+        <v>35.57</v>
       </c>
       <c r="G13" t="n">
-        <v>84.81999999999999</v>
+        <v>71</v>
       </c>
       <c r="H13" t="n">
-        <v>48.95</v>
+        <v>50.11</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Super Investor Stats:</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -2123,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>108.01</v>
+        <v>112.64</v>
       </c>
       <c r="P13" t="n">
-        <v>0.57</v>
+        <v>0.7</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -2137,15 +2137,15 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AltaRock Partners, Bill Ackman - Pershing Square Capital Management, Bill Nygren - Oakmark Select Fund, Chase Coleman - Tiger Global Management, Chris Hohn - TCI Fund Management, Christopher Davis - Davis Advisors, David Abrams - Abrams Capital Management, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Dodge &amp; Cox</t>
+          <t>Francois Rochon - Giverny Capital, Polen Capital Management, Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -2153,13 +2153,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>3.91</v>
+        <v>28.3</v>
       </c>
       <c r="G14" t="n">
-        <v>17.78</v>
+        <v>84.81999999999999</v>
       </c>
       <c r="H14" t="n">
-        <v>3.77</v>
+        <v>48.95</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -2174,7 +2174,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2186,10 +2186,10 @@
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>106.71</v>
+        <v>108.01</v>
       </c>
       <c r="P14" t="n">
-        <v>0.82</v>
+        <v>0.57</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -2200,15 +2200,15 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>HTZWW</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Daniel Loeb - Third Point, Francis Chou - Chou Associates</t>
+          <t>AltaRock Partners, Bill Ackman - Pershing Square Capital Management, Bill Nygren - Oakmark Select Fund, Chase Coleman - Tiger Global Management, Chris Hohn - TCI Fund Management, Christopher Davis - Davis Advisors, David Abrams - Abrams Capital Management, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Dodge &amp; Cox</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -2216,13 +2216,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>33.07</v>
+        <v>3.91</v>
       </c>
       <c r="G15" t="n">
-        <v>66</v>
+        <v>17.78</v>
       </c>
       <c r="H15" t="n">
-        <v>46.57</v>
+        <v>3.77</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Super Investor Stats:</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -2249,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>105.14</v>
+        <v>106.71</v>
       </c>
       <c r="P15" t="n">
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
@@ -2531,13 +2531,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>30.28</v>
+        <v>30.27</v>
       </c>
       <c r="G20" t="n">
-        <v>59.68</v>
+        <v>59.65</v>
       </c>
       <c r="H20" t="n">
-        <v>41.57</v>
+        <v>41.55</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -2564,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>96.40000000000001</v>
+        <v>96.36</v>
       </c>
       <c r="P20" t="n">
         <v>0.71</v>
@@ -2767,15 +2767,15 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>FIX</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AKO Capital, AltaRock Partners, Chris Hohn - TCI Fund Management, Chuck Akre - Akre Capital Management, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, John Armitage - Egerton Capital, Lindsell Train</t>
+          <t>Polen Capital Management, Thomas Gayner - Markel Group</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -2783,13 +2783,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>4.7</v>
+        <v>28.01</v>
       </c>
       <c r="G24" t="n">
-        <v>13.44</v>
+        <v>55.98</v>
       </c>
       <c r="H24" t="n">
-        <v>3.57</v>
+        <v>39.56</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2816,10 +2816,10 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>88.12</v>
+        <v>90.01000000000001</v>
       </c>
       <c r="P24" t="n">
-        <v>1.03</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
@@ -2830,15 +2830,15 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>FIX</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Polen Capital Management, Thomas Gayner - Markel Group</t>
+          <t>AKO Capital, AltaRock Partners, Chris Hohn - TCI Fund Management, Chuck Akre - Akre Capital Management, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, John Armitage - Egerton Capital, Lindsell Train</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2846,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>27.35</v>
+        <v>4.62</v>
       </c>
       <c r="G25" t="n">
-        <v>54.66</v>
+        <v>13.44</v>
       </c>
       <c r="H25" t="n">
-        <v>38.62</v>
+        <v>3.62</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2879,10 +2879,10 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>88.03</v>
+        <v>87.95999999999999</v>
       </c>
       <c r="P25" t="n">
-        <v>0.6899999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -3224,10 +3224,10 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>30.25</v>
+        <v>28.22</v>
       </c>
       <c r="G31" t="n">
-        <v>30.25</v>
+        <v>28.22</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3257,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>78.62</v>
+        <v>73.55</v>
       </c>
       <c r="P31" t="n">
-        <v>30.25</v>
+        <v>28.22</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -3271,15 +3271,15 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>RHI</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Greenhaven Associates</t>
+          <t>Christopher Bloomstran - Semper Augustus, Hillman Value Fund, Jensen Investment Management, Lindsell Train, Polen Capital Management, Robert Olstein - Olstein Capital Management, Terry Smith - Fundsmith, Thomas Gayner - Markel Group, Viking Global Investors</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3287,13 +3287,13 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>26.33</v>
+        <v>7.03</v>
       </c>
       <c r="G32" t="n">
-        <v>26.33</v>
+        <v>54.37</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>17.77</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -3320,10 +3320,10 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>68.81999999999999</v>
+        <v>68.23999999999999</v>
       </c>
       <c r="P32" t="n">
-        <v>26.33</v>
+        <v>0.37</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
@@ -3334,15 +3334,15 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Christopher Bloomstran - Semper Augustus, Hillman Value Fund, Jensen Investment Management, Lindsell Train, Polen Capital Management, Robert Olstein - Olstein Capital Management, Terry Smith - Fundsmith, Thomas Gayner - Markel Group, Viking Global Investors</t>
+          <t>AltaRock Partners, Chuck Akre - Akre Capital Management, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Guy Spier - Aquamarine Capital, Jensen Investment Management, John Armitage - Egerton Capital, Polen Capital Management, Terry Smith - Fundsmith, Thomas Gayner - Markel Group</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3350,13 +3350,13 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>7.03</v>
+        <v>5.32</v>
       </c>
       <c r="G33" t="n">
-        <v>54.37</v>
+        <v>18.54</v>
       </c>
       <c r="H33" t="n">
-        <v>17.77</v>
+        <v>6.24</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -3383,10 +3383,10 @@
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>68.23999999999999</v>
+        <v>67.91</v>
       </c>
       <c r="P33" t="n">
-        <v>0.37</v>
+        <v>0.73</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -3397,15 +3397,15 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>RHI</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AltaRock Partners, Chuck Akre - Akre Capital Management, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Guy Spier - Aquamarine Capital, Jensen Investment Management, John Armitage - Egerton Capital, Polen Capital Management, Terry Smith - Fundsmith, Thomas Gayner - Markel Group</t>
+          <t>Greenhaven Associates</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3413,13 +3413,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>5.32</v>
+        <v>25.9</v>
       </c>
       <c r="G34" t="n">
-        <v>18.54</v>
+        <v>25.9</v>
       </c>
       <c r="H34" t="n">
-        <v>6.24</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -3446,10 +3446,10 @@
         <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>67.91</v>
+        <v>67.75</v>
       </c>
       <c r="P34" t="n">
-        <v>0.73</v>
+        <v>25.9</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -3586,15 +3586,15 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>MRKR</t>
+          <t>COF</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>David Katz - Matrix Asset Advisors</t>
+          <t>Bill Nygren - Oakmark Select Fund, Christopher Davis - Davis Advisors, Clifford Sosin - CAS Investment Partners, Daniel Loeb - Third Point, David Katz - Matrix Asset Advisors, Dodge &amp; Cox, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Harry Burn - Sound Shore, John Armitage - Egerton Capital</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3602,13 +3602,13 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>25</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -3635,10 +3635,10 @@
         <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>65.5</v>
+        <v>64.65000000000001</v>
       </c>
       <c r="P37" t="n">
-        <v>25</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3649,15 +3649,15 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>SAIA</t>
+          <t>TDG</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Polen Capital Management</t>
+          <t>AltaRock Partners, Bryan Lawrence - Oakcliff Capital, Triple Frond Partners</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3665,13 +3665,13 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>24.7</v>
+        <v>20</v>
       </c>
       <c r="G38" t="n">
-        <v>24.7</v>
+        <v>27.26</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>6.34</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Industrial Goods</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -3698,10 +3698,10 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>64.75</v>
+        <v>62.63</v>
       </c>
       <c r="P38" t="n">
-        <v>24.7</v>
+        <v>2.72</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -3712,15 +3712,15 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>COF</t>
+          <t>SAIA</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Bill Nygren - Oakmark Select Fund, Christopher Davis - Davis Advisors, Clifford Sosin - CAS Investment Partners, Daniel Loeb - Third Point, David Katz - Matrix Asset Advisors, Dodge &amp; Cox, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Harry Burn - Sound Shore, John Armitage - Egerton Capital</t>
+          <t>Polen Capital Management</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3728,13 +3728,13 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>22.73</v>
       </c>
       <c r="G39" t="n">
-        <v>9.300000000000001</v>
+        <v>22.73</v>
       </c>
       <c r="H39" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3761,10 +3761,10 @@
         <v>0</v>
       </c>
       <c r="O39" t="n">
-        <v>64.65000000000001</v>
+        <v>59.82</v>
       </c>
       <c r="P39" t="n">
-        <v>0.8100000000000001</v>
+        <v>22.73</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
@@ -3775,15 +3775,15 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>TDG</t>
+          <t>MCO</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AltaRock Partners, Bryan Lawrence - Oakcliff Capital, Triple Frond Partners</t>
+          <t>AKO Capital, AltaRock Partners, Chris Hohn - TCI Fund Management, Chuck Akre - Akre Capital Management, Francis Chou - Chou Associates, Glenn Greenberg - Brave Warrior Advisors, Guy Spier - Aquamarine Capital, Lee Ainslie - Maverick Capital, Thomas Gayner - Markel Group, Triple Frond Partners</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3791,13 +3791,13 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>20</v>
+        <v>5.04</v>
       </c>
       <c r="G40" t="n">
-        <v>27.26</v>
+        <v>14.13</v>
       </c>
       <c r="H40" t="n">
-        <v>6.34</v>
+        <v>5.04</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -3812,7 +3812,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Industrial Goods</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -3824,10 +3824,10 @@
         <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>62.63</v>
+        <v>59.14</v>
       </c>
       <c r="P40" t="n">
-        <v>2.72</v>
+        <v>0.83</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
@@ -3838,15 +3838,15 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>MCO</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AKO Capital, AltaRock Partners, Chris Hohn - TCI Fund Management, Chuck Akre - Akre Capital Management, Francis Chou - Chou Associates, Glenn Greenberg - Brave Warrior Advisors, Guy Spier - Aquamarine Capital, Lee Ainslie - Maverick Capital, Thomas Gayner - Markel Group, Triple Frond Partners</t>
+          <t>Christopher Bloomstran - Semper Augustus, Duan Yongping - H&amp;H International Investment, First Eagle Investment Management, Francois Rochon - Giverny Capital, Harry Burn - Sound Shore, Hillman Value Fund, Kahn Brothers Group, Lindsell Train, Robert Olstein - Olstein Capital Management, Thomas Gayner - Markel Group</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -3854,13 +3854,13 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>5.04</v>
+        <v>5.17</v>
       </c>
       <c r="G41" t="n">
-        <v>14.13</v>
+        <v>17.59</v>
       </c>
       <c r="H41" t="n">
-        <v>5.04</v>
+        <v>5.67</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -3887,10 +3887,10 @@
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>59.14</v>
+        <v>58.14</v>
       </c>
       <c r="P41" t="n">
-        <v>0.83</v>
+        <v>0.78</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
@@ -3901,15 +3901,15 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>TSM</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Christopher Bloomstran - Semper Augustus, Duan Yongping - H&amp;H International Investment, First Eagle Investment Management, Francois Rochon - Giverny Capital, Harry Burn - Sound Shore, Hillman Value Fund, Kahn Brothers Group, Lindsell Train, Robert Olstein - Olstein Capital Management, Thomas Gayner - Markel Group</t>
+          <t>Chase Coleman - Tiger Global Management, Daniel Loeb - Third Point, David Rolfe - Wedgewood Partners, David Tepper - Appaloosa Management, Dodge &amp; Cox, Duan Yongping - H&amp;H International Investment, First Eagle Investment Management, Francois Rochon - Giverny Capital, Jensen Investment Management, Lee Ainslie - Maverick Capital</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -3917,13 +3917,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>5.17</v>
+        <v>2.62</v>
       </c>
       <c r="G42" t="n">
-        <v>17.59</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="H42" t="n">
-        <v>5.67</v>
+        <v>2.49</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -3950,10 +3950,10 @@
         <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>58.14</v>
+        <v>57.89</v>
       </c>
       <c r="P42" t="n">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -3964,15 +3964,15 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>TSM</t>
+          <t>PYPL</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Chase Coleman - Tiger Global Management, Daniel Loeb - Third Point, David Rolfe - Wedgewood Partners, David Tepper - Appaloosa Management, Dodge &amp; Cox, Duan Yongping - H&amp;H International Investment, First Eagle Investment Management, Francois Rochon - Giverny Capital, Jensen Investment Management, Lee Ainslie - Maverick Capital</t>
+          <t>David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Francis Chou - Chou Associates, Harry Burn - Sound Shore, Lee Ainslie - Maverick Capital, Lindsell Train, Mason Hawkins - Longleaf Partners, Pat Dorsey - Dorsey Asset Management, Polen Capital Management</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -3980,13 +3980,13 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>2.62</v>
+        <v>7.02</v>
       </c>
       <c r="G43" t="n">
-        <v>9.289999999999999</v>
+        <v>33.57</v>
       </c>
       <c r="H43" t="n">
-        <v>2.49</v>
+        <v>10.29</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -4013,10 +4013,10 @@
         <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>57.89</v>
+        <v>57.82</v>
       </c>
       <c r="P43" t="n">
-        <v>0.75</v>
+        <v>0.62</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
@@ -4027,15 +4027,15 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>PYPL</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, Francis Chou - Chou Associates, Harry Burn - Sound Shore, Lee Ainslie - Maverick Capital, Lindsell Train, Mason Hawkins - Longleaf Partners, Pat Dorsey - Dorsey Asset Management, Polen Capital Management</t>
+          <t>Chase Coleman - Tiger Global Management, Christopher Davis - Davis Advisors, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, David Tepper - Appaloosa Management, Dodge &amp; Cox, First Eagle Investment Management, Glenn Greenberg - Brave Warrior Advisors, Jensen Investment Management, Lee Ainslie - Maverick Capital</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4043,13 +4043,13 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>7.02</v>
+        <v>1.76</v>
       </c>
       <c r="G44" t="n">
-        <v>33.57</v>
+        <v>5.93</v>
       </c>
       <c r="H44" t="n">
-        <v>10.29</v>
+        <v>1.75</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -4076,10 +4076,10 @@
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>57.82</v>
+        <v>57.48</v>
       </c>
       <c r="P44" t="n">
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -4090,7 +4090,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>RH</t>
+          <t>AMRK</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Christopher Davis - Davis Advisors</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -4106,10 +4106,10 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>21.81</v>
+        <v>21.74</v>
       </c>
       <c r="G45" t="n">
-        <v>21.81</v>
+        <v>21.74</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -4139,10 +4139,10 @@
         <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>57.52</v>
+        <v>57.35</v>
       </c>
       <c r="P45" t="n">
-        <v>21.81</v>
+        <v>21.74</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
@@ -4153,15 +4153,15 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>CHTR</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Chase Coleman - Tiger Global Management, Christopher Davis - Davis Advisors, David Katz - Matrix Asset Advisors, David Rolfe - Wedgewood Partners, David Tepper - Appaloosa Management, Dodge &amp; Cox, First Eagle Investment Management, Glenn Greenberg - Brave Warrior Advisors, Jensen Investment Management, Lee Ainslie - Maverick Capital</t>
+          <t>Bill Nygren - Oakmark Select Fund, Bryan Lawrence - Oakcliff Capital, Dodge &amp; Cox, First Eagle Investment Management, Richard Pzena - Hancock Classic Value, Ruane Cunniff - Sequoia Fund, Steven Romick - FPA Crescent Fund, Tom Bancroft - Makaira Partners, Triple Frond Partners, Wallace Weitz - Weitz Large Cap Equity Fund</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -4169,13 +4169,13 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>1.76</v>
+        <v>5.07</v>
       </c>
       <c r="G46" t="n">
-        <v>5.93</v>
+        <v>24.73</v>
       </c>
       <c r="H46" t="n">
-        <v>1.75</v>
+        <v>7</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -4190,7 +4190,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
@@ -4202,10 +4202,10 @@
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>57.48</v>
+        <v>55.5</v>
       </c>
       <c r="P46" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
@@ -4216,7 +4216,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>AMRK</t>
+          <t>RH</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Christopher Davis - Davis Advisors</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -4232,10 +4232,10 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="G47" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
@@ -4265,10 +4265,10 @@
         <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>57.35</v>
+        <v>54.38</v>
       </c>
       <c r="P47" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -4279,15 +4279,15 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>CHTR</t>
+          <t>EQH</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Bill Nygren - Oakmark Select Fund, Bryan Lawrence - Oakcliff Capital, Dodge &amp; Cox, First Eagle Investment Management, Richard Pzena - Hancock Classic Value, Ruane Cunniff - Sequoia Fund, Steven Romick - FPA Crescent Fund, Tom Bancroft - Makaira Partners, Triple Frond Partners, Wallace Weitz - Weitz Large Cap Equity Fund</t>
+          <t>Greg Alexander - Conifer Management, Lee Ainslie - Maverick Capital, Richard Pzena - Hancock Classic Value, Viking Global Investors</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
@@ -4295,13 +4295,13 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>5.07</v>
+        <v>10.54</v>
       </c>
       <c r="G48" t="n">
-        <v>24.73</v>
+        <v>39.48</v>
       </c>
       <c r="H48" t="n">
-        <v>7</v>
+        <v>19.31</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -4328,10 +4328,10 @@
         <v>0</v>
       </c>
       <c r="O48" t="n">
-        <v>55.5</v>
+        <v>52.82</v>
       </c>
       <c r="P48" t="n">
-        <v>0.63</v>
+        <v>0.52</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
@@ -4342,7 +4342,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>EQH</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Greg Alexander - Conifer Management, Lee Ainslie - Maverick Capital, Richard Pzena - Hancock Classic Value, Viking Global Investors</t>
+          <t>AKO Capital, AltaRock Partners, Lindsell Train, Valley Forge Capital Management</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
@@ -4358,13 +4358,13 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>10.54</v>
+        <v>12.04</v>
       </c>
       <c r="G49" t="n">
-        <v>39.48</v>
+        <v>32.29</v>
       </c>
       <c r="H49" t="n">
-        <v>19.31</v>
+        <v>14.44</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -4391,10 +4391,10 @@
         <v>0</v>
       </c>
       <c r="O49" t="n">
-        <v>52.82</v>
+        <v>52.22</v>
       </c>
       <c r="P49" t="n">
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
@@ -4405,15 +4405,15 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>FICO</t>
+          <t>OLLI</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AKO Capital, AltaRock Partners, Lindsell Train, Valley Forge Capital Management</t>
+          <t>Lee Ainslie - Maverick Capital, Polen Capital Management</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
@@ -4421,13 +4421,13 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>12.04</v>
+        <v>14.38</v>
       </c>
       <c r="G50" t="n">
-        <v>32.29</v>
+        <v>28.6</v>
       </c>
       <c r="H50" t="n">
-        <v>14.44</v>
+        <v>20.12</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -4454,10 +4454,10 @@
         <v>0</v>
       </c>
       <c r="O50" t="n">
-        <v>52.22</v>
+        <v>49.06</v>
       </c>
       <c r="P50" t="n">
-        <v>0.78</v>
+        <v>0.68</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
@@ -4468,7 +4468,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>OLLI</t>
+          <t>ORLA</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Lee Ainslie - Maverick Capital, Polen Capital Management</t>
+          <t>First Eagle Investment Management, Prem Watsa - Fairfax Financial Holdings</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
@@ -4484,13 +4484,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>14.38</v>
+        <v>14.36</v>
       </c>
       <c r="G51" t="n">
-        <v>28.6</v>
+        <v>28.57</v>
       </c>
       <c r="H51" t="n">
-        <v>20.12</v>
+        <v>20.09</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Materials</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
       <c r="O51" t="n">
-        <v>49.06</v>
+        <v>49</v>
       </c>
       <c r="P51" t="n">
         <v>0.68</v>
@@ -4531,15 +4531,15 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>ORLA</t>
+          <t>MRKR</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>First Eagle Investment Management, Prem Watsa - Fairfax Financial Holdings</t>
+          <t>David Katz - Matrix Asset Advisors</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -4547,13 +4547,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>14.36</v>
+        <v>18.33</v>
       </c>
       <c r="G52" t="n">
-        <v>28.57</v>
+        <v>18.33</v>
       </c>
       <c r="H52" t="n">
-        <v>20.09</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -4568,7 +4568,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -4580,10 +4580,10 @@
         <v>0</v>
       </c>
       <c r="O52" t="n">
-        <v>49</v>
+        <v>48.82</v>
       </c>
       <c r="P52" t="n">
-        <v>0.68</v>
+        <v>18.33</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5114,13 +5114,13 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>5.48</v>
+        <v>5.54</v>
       </c>
       <c r="G61" t="n">
         <v>20.32</v>
       </c>
       <c r="H61" t="n">
-        <v>7.26</v>
+        <v>7.21</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -5147,10 +5147,10 @@
         <v>0</v>
       </c>
       <c r="O61" t="n">
-        <v>45.12</v>
+        <v>45.24</v>
       </c>
       <c r="P61" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -5539,7 +5539,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>CATO</t>
+          <t>TRMD</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Howard Marks - Oaktree Capital Management</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
@@ -5555,10 +5555,10 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="G68" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -5588,10 +5588,10 @@
         <v>0</v>
       </c>
       <c r="O68" t="n">
-        <v>44.3</v>
+        <v>43.98</v>
       </c>
       <c r="P68" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
@@ -5602,15 +5602,15 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>TRMD</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Howard Marks - Oaktree Capital Management</t>
+          <t>Christopher Davis - Davis Advisors, David Katz - Matrix Asset Advisors, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Greenhaven Associates, Kahn Brothers Group, Mairs &amp; Power Growth Fund, Samantha McLemore - Patient Capital Management, Thomas Gayner - Markel Group, Thomas Russo - Gardner Russo &amp; Quinn</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
@@ -5618,13 +5618,13 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>16.39</v>
+        <v>1.59</v>
       </c>
       <c r="G69" t="n">
-        <v>16.39</v>
+        <v>5.9</v>
       </c>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
@@ -5651,10 +5651,10 @@
         <v>0</v>
       </c>
       <c r="O69" t="n">
-        <v>43.98</v>
+        <v>42.13</v>
       </c>
       <c r="P69" t="n">
-        <v>16.39</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
@@ -5665,15 +5665,15 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>IBKR</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Christopher Davis - Davis Advisors, David Katz - Matrix Asset Advisors, Francois Rochon - Giverny Capital, Glenn Greenberg - Brave Warrior Advisors, Greenhaven Associates, Kahn Brothers Group, Mairs &amp; Power Growth Fund, Samantha McLemore - Patient Capital Management, Thomas Gayner - Markel Group, Thomas Russo - Gardner Russo &amp; Quinn</t>
+          <t>Bryan Lawrence - Oakcliff Capital, John Armitage - Egerton Capital, Robert Vinall - RV Capital GmbH, William Von Mueffling - Cantillon Capital Management</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -5681,13 +5681,13 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>1.59</v>
+        <v>9.32</v>
       </c>
       <c r="G70" t="n">
-        <v>5.9</v>
+        <v>22.48</v>
       </c>
       <c r="H70" t="n">
-        <v>1.85</v>
+        <v>9</v>
       </c>
       <c r="I70" t="n">
         <v>0</v>
@@ -5714,10 +5714,10 @@
         <v>0</v>
       </c>
       <c r="O70" t="n">
-        <v>42.13</v>
+        <v>41.88</v>
       </c>
       <c r="P70" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
@@ -5728,15 +5728,15 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>IBKR</t>
+          <t>EXE</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Bryan Lawrence - Oakcliff Capital, John Armitage - Egerton Capital, Robert Vinall - RV Capital GmbH, William Von Mueffling - Cantillon Capital Management</t>
+          <t>Howard Marks - Oaktree Capital Management</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -5744,13 +5744,13 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>9.32</v>
+        <v>15.31</v>
       </c>
       <c r="G71" t="n">
-        <v>22.48</v>
+        <v>15.31</v>
       </c>
       <c r="H71" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
@@ -5765,7 +5765,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -5777,10 +5777,10 @@
         <v>0</v>
       </c>
       <c r="O71" t="n">
-        <v>41.88</v>
+        <v>41.28</v>
       </c>
       <c r="P71" t="n">
-        <v>0.93</v>
+        <v>15.31</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
@@ -5791,15 +5791,15 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>EXE</t>
+          <t>PDD</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Howard Marks - Oaktree Capital Management</t>
+          <t>Chase Coleman - Tiger Global Management, David Tepper - Appaloosa Management, Duan Yongping - H&amp;H International Investment, Norbert Lou - Punch Card Management, Polen Capital Management, Robert Vinall - RV Capital GmbH</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -5807,13 +5807,13 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>15.31</v>
+        <v>7.41</v>
       </c>
       <c r="G72" t="n">
-        <v>15.31</v>
+        <v>16.76</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>5.95</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
@@ -5828,7 +5828,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Consumer Goods</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
@@ -5840,10 +5840,10 @@
         <v>0</v>
       </c>
       <c r="O72" t="n">
-        <v>41.28</v>
+        <v>41.2</v>
       </c>
       <c r="P72" t="n">
-        <v>15.31</v>
+        <v>1.07</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
@@ -5854,15 +5854,15 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>PDD</t>
+          <t>APTV</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Chase Coleman - Tiger Global Management, David Tepper - Appaloosa Management, Duan Yongping - H&amp;H International Investment, Norbert Lou - Punch Card Management, Polen Capital Management, Robert Vinall - RV Capital GmbH</t>
+          <t>Alex Roepers - Atlantic Investment Management, Robert Olstein - Olstein Capital Management</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -5870,13 +5870,13 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>7.41</v>
+        <v>11.95</v>
       </c>
       <c r="G73" t="n">
-        <v>16.76</v>
+        <v>22.4</v>
       </c>
       <c r="H73" t="n">
-        <v>5.95</v>
+        <v>14.78</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
@@ -5903,10 +5903,10 @@
         <v>0</v>
       </c>
       <c r="O73" t="n">
-        <v>41.2</v>
+        <v>41.1</v>
       </c>
       <c r="P73" t="n">
-        <v>1.07</v>
+        <v>0.76</v>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
@@ -5917,15 +5917,15 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>APTV</t>
+          <t>SGOV</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Alex Roepers - Atlantic Investment Management, Robert Olstein - Olstein Capital Management</t>
+          <t>Christopher Bloomstran - Semper Augustus, Norbert Lou - Punch Card Management, Polen Capital Management</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
@@ -5933,13 +5933,13 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>11.95</v>
+        <v>9.06</v>
       </c>
       <c r="G74" t="n">
-        <v>22.4</v>
+        <v>27</v>
       </c>
       <c r="H74" t="n">
-        <v>14.78</v>
+        <v>15.54</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Consumer Goods</t>
+          <t>Super Investor Stats:</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
@@ -5966,10 +5966,10 @@
         <v>0</v>
       </c>
       <c r="O74" t="n">
-        <v>41.1</v>
+        <v>40.62</v>
       </c>
       <c r="P74" t="n">
-        <v>0.76</v>
+        <v>0.55</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
@@ -5980,15 +5980,15 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>SGOV</t>
+          <t>CATO</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Christopher Bloomstran - Semper Augustus, Norbert Lou - Punch Card Management, Polen Capital Management</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -5996,13 +5996,13 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>9.06</v>
+        <v>15.02</v>
       </c>
       <c r="G75" t="n">
-        <v>27</v>
+        <v>15.02</v>
       </c>
       <c r="H75" t="n">
-        <v>15.54</v>
+        <v>0</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Super Investor Stats:</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
@@ -6029,10 +6029,10 @@
         <v>0</v>
       </c>
       <c r="O75" t="n">
-        <v>40.62</v>
+        <v>40.55</v>
       </c>
       <c r="P75" t="n">
-        <v>0.55</v>
+        <v>15.02</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
@@ -8118,13 +8118,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>4.7</v>
+        <v>4.62</v>
       </c>
       <c r="G7" t="n">
         <v>13.44</v>
       </c>
       <c r="H7" t="n">
-        <v>3.57</v>
+        <v>3.62</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -8151,10 +8151,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>88.12</v>
+        <v>87.95999999999999</v>
       </c>
       <c r="P7" t="n">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -10323,13 +10323,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>5.48</v>
+        <v>5.54</v>
       </c>
       <c r="G42" t="n">
         <v>20.32</v>
       </c>
       <c r="H42" t="n">
-        <v>7.26</v>
+        <v>7.21</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -10356,10 +10356,10 @@
         <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>45.12</v>
+        <v>45.24</v>
       </c>
       <c r="P42" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -11610,15 +11610,15 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>PHJMF</t>
+          <t>HTZWW</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Thomas Russo - Gardner Russo &amp; Quinn</t>
+          <t>Daniel Loeb - Third Point, Francis Chou - Chou Associates</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -11626,13 +11626,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>33.33</v>
+        <v>35.57</v>
       </c>
       <c r="G11" t="n">
-        <v>33.33</v>
+        <v>71</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>50.11</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -11647,7 +11647,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Consumer Goods</t>
+          <t>Super Investor Stats:</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -11659,10 +11659,10 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>86.31999999999999</v>
+        <v>112.64</v>
       </c>
       <c r="P11" t="n">
-        <v>33.33</v>
+        <v>0.7</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -11673,15 +11673,15 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>HTZWW</t>
+          <t>PHJMF</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Daniel Loeb - Third Point, Francis Chou - Chou Associates</t>
+          <t>Thomas Russo - Gardner Russo &amp; Quinn</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -11689,13 +11689,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>33.07</v>
+        <v>33.33</v>
       </c>
       <c r="G12" t="n">
-        <v>66</v>
+        <v>33.33</v>
       </c>
       <c r="H12" t="n">
-        <v>46.57</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -11710,7 +11710,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Super Investor Stats:</t>
+          <t>Consumer Goods</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -11722,10 +11722,10 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>105.14</v>
+        <v>86.31999999999999</v>
       </c>
       <c r="P12" t="n">
-        <v>0.7</v>
+        <v>33.33</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -11878,13 +11878,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>30.28</v>
+        <v>30.27</v>
       </c>
       <c r="G15" t="n">
-        <v>59.68</v>
+        <v>59.65</v>
       </c>
       <c r="H15" t="n">
-        <v>41.57</v>
+        <v>41.55</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -11911,7 +11911,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>96.40000000000001</v>
+        <v>96.36</v>
       </c>
       <c r="P15" t="n">
         <v>0.71</v>
@@ -11988,15 +11988,15 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>SKIL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polen Capital Management</t>
+          <t>Francois Rochon - Giverny Capital, Polen Capital Management, Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -12004,13 +12004,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>30.25</v>
+        <v>28.3</v>
       </c>
       <c r="G17" t="n">
-        <v>30.25</v>
+        <v>84.81999999999999</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>48.95</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -12025,7 +12025,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -12037,10 +12037,10 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>78.62</v>
+        <v>108.01</v>
       </c>
       <c r="P17" t="n">
-        <v>30.25</v>
+        <v>0.57</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -12051,15 +12051,15 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>SKIL</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Francois Rochon - Giverny Capital, Polen Capital Management, Yacktman Asset Management</t>
+          <t>Polen Capital Management</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -12067,13 +12067,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>28.3</v>
+        <v>28.22</v>
       </c>
       <c r="G18" t="n">
-        <v>84.81999999999999</v>
+        <v>28.22</v>
       </c>
       <c r="H18" t="n">
-        <v>48.95</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -12088,7 +12088,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -12100,10 +12100,10 @@
         <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>108.01</v>
+        <v>73.55</v>
       </c>
       <c r="P18" t="n">
-        <v>0.57</v>
+        <v>28.22</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
@@ -12130,13 +12130,13 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>27.35</v>
+        <v>28.01</v>
       </c>
       <c r="G19" t="n">
-        <v>54.66</v>
+        <v>55.98</v>
       </c>
       <c r="H19" t="n">
-        <v>38.62</v>
+        <v>39.56</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -12163,7 +12163,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>88.03</v>
+        <v>90.01000000000001</v>
       </c>
       <c r="P19" t="n">
         <v>0.6899999999999999</v>
@@ -12256,10 +12256,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>26.33</v>
+        <v>25.9</v>
       </c>
       <c r="G21" t="n">
-        <v>26.33</v>
+        <v>25.9</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -12289,10 +12289,10 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>68.81999999999999</v>
+        <v>67.75</v>
       </c>
       <c r="P21" t="n">
-        <v>26.33</v>
+        <v>25.9</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -12303,7 +12303,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>MRKR</t>
+          <t>SAIA</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -12311,7 +12311,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>David Katz - Matrix Asset Advisors</t>
+          <t>Polen Capital Management</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -12319,10 +12319,10 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>25</v>
+        <v>22.73</v>
       </c>
       <c r="G22" t="n">
-        <v>25</v>
+        <v>22.73</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -12340,7 +12340,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -12352,10 +12352,10 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>65.5</v>
+        <v>59.82</v>
       </c>
       <c r="P22" t="n">
-        <v>25</v>
+        <v>22.73</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -12366,7 +12366,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>SAIA</t>
+          <t>AMRK</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -12374,7 +12374,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Polen Capital Management</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -12382,10 +12382,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>24.7</v>
+        <v>21.74</v>
       </c>
       <c r="G23" t="n">
-        <v>24.7</v>
+        <v>21.74</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -12403,7 +12403,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -12415,10 +12415,10 @@
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>64.75</v>
+        <v>57.35</v>
       </c>
       <c r="P23" t="n">
-        <v>24.7</v>
+        <v>21.74</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
@@ -12429,15 +12429,15 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>RH</t>
+          <t>HCC</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Christopher Davis - Davis Advisors</t>
+          <t>Mohnish Pabrai - Pabrai Investments, Third Avenue Management</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -12445,13 +12445,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>21.81</v>
+        <v>21.22</v>
       </c>
       <c r="G24" t="n">
-        <v>21.81</v>
+        <v>36.57</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>21.71</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -12466,7 +12466,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -12478,10 +12478,10 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>57.52</v>
+        <v>66.72</v>
       </c>
       <c r="P24" t="n">
-        <v>21.81</v>
+        <v>0.93</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
@@ -12492,7 +12492,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>AMRK</t>
+          <t>RH</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -12500,7 +12500,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Christopher Davis - Davis Advisors</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -12508,10 +12508,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="G25" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -12529,7 +12529,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -12541,10 +12541,10 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>57.35</v>
+        <v>54.38</v>
       </c>
       <c r="P25" t="n">
-        <v>21.74</v>
+        <v>20.55</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -12555,15 +12555,15 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>HCC</t>
+          <t>TDG</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Mohnish Pabrai - Pabrai Investments, Third Avenue Management</t>
+          <t>AltaRock Partners, Bryan Lawrence - Oakcliff Capital, Triple Frond Partners</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -12571,13 +12571,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>21.22</v>
+        <v>20</v>
       </c>
       <c r="G26" t="n">
-        <v>36.57</v>
+        <v>27.26</v>
       </c>
       <c r="H26" t="n">
-        <v>21.71</v>
+        <v>6.34</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -12592,7 +12592,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Industrial Goods</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -12604,10 +12604,10 @@
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>66.72</v>
+        <v>62.63</v>
       </c>
       <c r="P26" t="n">
-        <v>0.93</v>
+        <v>2.72</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -12618,15 +12618,15 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>TDG</t>
+          <t>MRKR</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AltaRock Partners, Bryan Lawrence - Oakcliff Capital, Triple Frond Partners</t>
+          <t>David Katz - Matrix Asset Advisors</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -12634,13 +12634,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>20</v>
+        <v>18.33</v>
       </c>
       <c r="G27" t="n">
-        <v>27.26</v>
+        <v>18.33</v>
       </c>
       <c r="H27" t="n">
-        <v>6.34</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -12655,7 +12655,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Industrial Goods</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -12667,10 +12667,10 @@
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>62.63</v>
+        <v>48.82</v>
       </c>
       <c r="P27" t="n">
-        <v>2.72</v>
+        <v>18.33</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
@@ -12870,7 +12870,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>CATO</t>
+          <t>TRMD</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -12878,7 +12878,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Howard Marks - Oaktree Capital Management</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -12886,10 +12886,10 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="G31" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -12907,7 +12907,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -12919,10 +12919,10 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>44.3</v>
+        <v>43.98</v>
       </c>
       <c r="P31" t="n">
-        <v>16.52</v>
+        <v>16.39</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -12933,7 +12933,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>TRMD</t>
+          <t>EXE</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -12949,10 +12949,10 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>16.39</v>
+        <v>15.31</v>
       </c>
       <c r="G32" t="n">
-        <v>16.39</v>
+        <v>15.31</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -12970,7 +12970,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -12982,10 +12982,10 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>43.98</v>
+        <v>41.28</v>
       </c>
       <c r="P32" t="n">
-        <v>16.39</v>
+        <v>15.31</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
@@ -12996,15 +12996,15 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>EXE</t>
+          <t>GTLS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Howard Marks - Oaktree Capital Management</t>
+          <t>Alex Roepers - Atlantic Investment Management, Glenn Welling - Engaged Capital</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -13012,13 +13012,13 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>15.31</v>
+        <v>15.08</v>
       </c>
       <c r="G33" t="n">
-        <v>15.31</v>
+        <v>16.57</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>2.11</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -13033,7 +13033,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Industrial Goods</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -13045,10 +13045,10 @@
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>41.28</v>
+        <v>44.44</v>
       </c>
       <c r="P33" t="n">
-        <v>15.31</v>
+        <v>4.85</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -13059,15 +13059,15 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>GTLS</t>
+          <t>CATO</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Alex Roepers - Atlantic Investment Management, Glenn Welling - Engaged Capital</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -13075,13 +13075,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>15.08</v>
+        <v>15.02</v>
       </c>
       <c r="G34" t="n">
-        <v>16.57</v>
+        <v>15.02</v>
       </c>
       <c r="H34" t="n">
-        <v>2.11</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -13096,7 +13096,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Industrial Goods</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -13108,10 +13108,10 @@
         <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>44.44</v>
+        <v>40.55</v>
       </c>
       <c r="P34" t="n">
-        <v>4.85</v>
+        <v>15.02</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -14468,21 +14468,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>2078</v>
+        <v>1042</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Polen Capital Management</t>
+          <t>Francis Chou - Chou Associates</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>TTEK</t>
+          <t>HTZWW</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>67.42</v>
+        <v>71</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -14500,7 +14500,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Super Investor Stats:</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -14509,21 +14509,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1042</v>
+        <v>2078</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Francis Chou - Chou Associates</t>
+          <t>Polen Capital Management</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HTZWW</t>
+          <t>TTEK</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>66</v>
+        <v>67.42</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -14541,7 +14541,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Super Investor Stats:</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -14687,7 +14687,7 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>59.68</v>
+        <v>59.65</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -14769,7 +14769,7 @@
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>54.66</v>
+        <v>55.98</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -15411,7 +15411,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>2076</v>
+        <v>2072</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -15420,12 +15420,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SKIL</t>
+          <t>OLLI</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>30.25</v>
+        <v>28.6</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -15443,7 +15443,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K30" t="n">
@@ -15452,21 +15452,21 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>2072</v>
+        <v>2081</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Polen Capital Management</t>
+          <t>Prem Watsa - Fairfax Financial Holdings</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OLLI</t>
+          <t>ORLA</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>28.6</v>
+        <v>28.57</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -15484,7 +15484,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Materials</t>
         </is>
       </c>
       <c r="K31" t="n">
@@ -15493,21 +15493,21 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Prem Watsa - Fairfax Financial Holdings</t>
+          <t>Polen Capital Management</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ORLA</t>
+          <t>SKIL</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>28.57</v>
+        <v>28.22</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -15525,7 +15525,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="K32" t="n">
@@ -15657,21 +15657,21 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>1166</v>
+        <v>1769</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Greenhaven Associates</t>
+          <t>Li Lu - Himalaya Capital Management</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RHI</t>
+          <t>BAC</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>26.33</v>
+        <v>26.12</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -15689,7 +15689,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K36" t="n">
@@ -15698,21 +15698,21 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>1769</v>
+        <v>1166</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Li Lu - Himalaya Capital Management</t>
+          <t>Greenhaven Associates</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BAC</t>
+          <t>RHI</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>26.12</v>
+        <v>25.9</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -15730,7 +15730,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="K37" t="n">
@@ -15903,21 +15903,21 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>606</v>
+        <v>2731</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>David Katz - Matrix Asset Advisors</t>
+          <t>Tom Bancroft - Makaira Partners</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MRKR</t>
+          <t>CHTR</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>25</v>
+        <v>24.73</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -15935,7 +15935,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K42" t="n">
@@ -15944,21 +15944,21 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>2731</v>
+        <v>1936</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Tom Bancroft - Makaira Partners</t>
+          <t>Mohnish Pabrai - Pabrai Investments</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CHTR</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>24.73</v>
+        <v>23.87</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -15976,7 +15976,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="K43" t="n">
@@ -15999,7 +15999,7 @@
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>24.7</v>
+        <v>22.73</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -16026,21 +16026,21 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1936</v>
+        <v>148</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mohnish Pabrai - Pabrai Investments</t>
+          <t>Bryan Lawrence - Oakcliff Capital</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>IBKR</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>23.87</v>
+        <v>22.48</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -16058,7 +16058,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K45" t="n">
@@ -16067,21 +16067,21 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Bryan Lawrence - Oakcliff Capital</t>
+          <t>Alex Roepers - Atlantic Investment Management</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>IBKR</t>
+          <t>APTV</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>22.48</v>
+        <v>22.4</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -16099,7 +16099,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Consumer Goods</t>
         </is>
       </c>
       <c r="K46" t="n">
@@ -16108,21 +16108,21 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>26</v>
+        <v>1169</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Alex Roepers - Atlantic Investment Management</t>
+          <t>Greg Alexander - Conifer Management</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>APTV</t>
+          <t>LAD</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>22.4</v>
+        <v>22.25</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -16140,7 +16140,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Consumer Goods</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K47" t="n">
@@ -16149,21 +16149,21 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1169</v>
+        <v>1937</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Greg Alexander - Conifer Management</t>
+          <t>Mohnish Pabrai - Pabrai Investments</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>LAD</t>
+          <t>AMR</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>22.25</v>
+        <v>22.11</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -16181,7 +16181,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Materials</t>
         </is>
       </c>
       <c r="K48" t="n">
@@ -16190,21 +16190,21 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1937</v>
+        <v>243</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mohnish Pabrai - Pabrai Investments</t>
+          <t>Chris Hohn - TCI Fund Management</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>AMR</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>22.11</v>
+        <v>21.95</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -16222,7 +16222,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="K49" t="n">
@@ -16231,21 +16231,21 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>243</v>
+        <v>627</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Chris Hohn - TCI Fund Management</t>
+          <t>David Tepper - Appaloosa Management</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>BABA</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>21.95</v>
+        <v>21.92</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -16263,7 +16263,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="K50" t="n">
@@ -16272,21 +16272,21 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>627</v>
+        <v>45</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>David Tepper - Appaloosa Management</t>
+          <t>Bill &amp; Melinda Gates Foundation Trust</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BABA</t>
+          <t>BRK.B</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>21.92</v>
+        <v>21.88</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -16304,7 +16304,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K51" t="n">
@@ -16313,21 +16313,21 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>45</v>
+        <v>3218</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Bill &amp; Melinda Gates Foundation Trust</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BRK.B</t>
+          <t>AMRK</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>21.88</v>
+        <v>21.74</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -16354,21 +16354,21 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>391</v>
+        <v>1132</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Christopher Davis - Davis Advisors</t>
+          <t>Glenn Welling - Engaged Capital</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>RH</t>
+          <t>VFC</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>21.81</v>
+        <v>21.7</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -16386,7 +16386,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K53" t="n">
@@ -16395,21 +16395,21 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>3218</v>
+        <v>1770</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Li Lu - Himalaya Capital Management</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>AMRK</t>
+          <t>BRK.B</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>21.74</v>
+        <v>21.61</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -16436,21 +16436,21 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1132</v>
+        <v>1940</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Glenn Welling - Engaged Capital</t>
+          <t>Nelson Peltz - Trian Fund Management</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>VFC</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>21.7</v>
+        <v>21.59</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="K55" t="n">
@@ -16477,21 +16477,21 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>1770</v>
+        <v>1465</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Li Lu - Himalaya Capital Management</t>
+          <t>Josh Tarasoff - Greenlea Lane Capital</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BRK.B</t>
+          <t>AMZN</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>21.61</v>
+        <v>21.34</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -16509,7 +16509,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K56" t="n">
@@ -16518,21 +16518,21 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>1940</v>
+        <v>391</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Nelson Peltz - Trian Fund Management</t>
+          <t>Christopher Davis - Davis Advisors</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>RH</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>21.59</v>
+        <v>20.55</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -16550,7 +16550,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K57" t="n">
@@ -16559,21 +16559,21 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>1465</v>
+        <v>253</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Josh Tarasoff - Greenlea Lane Capital</t>
+          <t>Christopher Bloomstran - Semper Augustus</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>BRK.B</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>21.34</v>
+        <v>20.55</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -16591,7 +16591,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K58" t="n">
@@ -16600,21 +16600,21 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>253</v>
+        <v>2845</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Christopher Bloomstran - Semper Augustus</t>
+          <t>Triple Frond Partners</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BRK.B</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>20.55</v>
+        <v>20.45</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -16632,7 +16632,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="K59" t="n">
@@ -16641,21 +16641,21 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>2845</v>
+        <v>2940</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Triple Frond Partners</t>
+          <t>Valley Forge Capital Management</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>SPGI</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>20.45</v>
+        <v>20.32</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -16673,7 +16673,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K60" t="n">
@@ -16682,21 +16682,21 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>2940</v>
+        <v>36</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Valley Forge Capital Management</t>
+          <t>AltaRock Partners</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SPGI</t>
+          <t>AMZN</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>20.32</v>
+        <v>19.9</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -16723,7 +16723,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -16732,12 +16732,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>19.9</v>
+        <v>19.46</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -16755,7 +16755,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="K62" t="n">
@@ -16764,21 +16764,21 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>37</v>
+        <v>1173</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>AltaRock Partners</t>
+          <t>Guy Spier - Aquamarine Capital</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>19.46</v>
+        <v>19.24</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -16796,7 +16796,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K63" t="n">
@@ -16805,21 +16805,21 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1173</v>
+        <v>1141</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Guy Spier - Aquamarine Capital</t>
+          <t>Greenhaven Associates</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>19.24</v>
+        <v>18.8</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -16846,21 +16846,21 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>1141</v>
+        <v>2941</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Greenhaven Associates</t>
+          <t>Valley Forge Capital Management</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>18.8</v>
+        <v>18.54</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -16878,7 +16878,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K65" t="n">
@@ -16887,21 +16887,21 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>2941</v>
+        <v>69</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Valley Forge Capital Management</t>
+          <t>Bill Ackman - Pershing Square Capital Management</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>UBER</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>18.54</v>
+        <v>18.5</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -16919,7 +16919,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="K66" t="n">
@@ -16928,21 +16928,21 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>69</v>
+        <v>1466</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Bill Ackman - Pershing Square Capital Management</t>
+          <t>Josh Tarasoff - Greenlea Lane Capital</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>UBER</t>
+          <t>BRK.A</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>18.5</v>
+        <v>18.48</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -16960,7 +16960,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>Financials</t>
         </is>
       </c>
       <c r="K67" t="n">
@@ -16969,21 +16969,21 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1466</v>
+        <v>606</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Josh Tarasoff - Greenlea Lane Capital</t>
+          <t>David Katz - Matrix Asset Advisors</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BRK.A</t>
+          <t>MRKR</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>18.48</v>
+        <v>18.33</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -17001,7 +17001,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Financials</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="K68" t="n">
@@ -17707,21 +17707,21 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>2732</v>
+        <v>389</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Tom Bancroft - Makaira Partners</t>
+          <t>Christopher Davis - Davis Advisors</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>BBWI</t>
+          <t>CCK</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="n">
-        <v>16.66</v>
+        <v>16.7</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -17739,7 +17739,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Consumer Goods</t>
         </is>
       </c>
       <c r="K86" t="n">
@@ -17748,21 +17748,21 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>1133</v>
+        <v>2732</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Glenn Welling - Engaged Capital</t>
+          <t>Tom Bancroft - Makaira Partners</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>PTLO</t>
+          <t>BBWI</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>16.61</v>
+        <v>16.66</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -17780,7 +17780,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Consumer Cyclical</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K87" t="n">
@@ -17789,21 +17789,21 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>28</v>
+        <v>1133</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Alex Roepers - Atlantic Investment Management</t>
+          <t>Glenn Welling - Engaged Capital</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>GTLS</t>
+          <t>PTLO</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
-        <v>16.57</v>
+        <v>16.61</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -17821,7 +17821,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Industrial Goods</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="K88" t="n">
@@ -17830,21 +17830,21 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>3219</v>
+        <v>28</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Alex Roepers - Atlantic Investment Management</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>CATO</t>
+          <t>GTLS</t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
-        <v>16.52</v>
+        <v>16.57</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
@@ -17862,7 +17862,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Industrial Goods</t>
         </is>
       </c>
       <c r="K89" t="n">
@@ -17912,21 +17912,21 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>389</v>
+        <v>3114</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Christopher Davis - Davis Advisors</t>
+          <t>Warren Buffett - Berkshire Hathaway</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>CCK</t>
+          <t>BATRK</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="n">
-        <v>16.37</v>
+        <v>16.22</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -17944,7 +17944,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Consumer Goods</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="K91" t="n">
@@ -18117,21 +18117,21 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>3114</v>
+        <v>149</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Warren Buffett - Berkshire Hathaway</t>
+          <t>Bryan Lawrence - Oakcliff Capital</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>BATRK</t>
+          <t>TDG</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="n">
-        <v>15.67</v>
+        <v>15.52</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -18149,7 +18149,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Industrial Goods</t>
         </is>
       </c>
       <c r="K96" t="n">
@@ -18158,21 +18158,21 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>149</v>
+        <v>1260</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Bryan Lawrence - Oakcliff Capital</t>
+          <t>Howard Marks - Oaktree Capital Management</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>TDG</t>
+          <t>EXE</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
-        <v>15.52</v>
+        <v>15.31</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -18190,7 +18190,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Industrial Goods</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="K97" t="n">
@@ -18240,21 +18240,21 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>1260</v>
+        <v>1953</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Howard Marks - Oaktree Capital Management</t>
+          <t>Pat Dorsey - Dorsey Asset Management</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>EXE</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
-        <v>15.31</v>
+        <v>15.17</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -18272,7 +18272,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K99" t="n">
@@ -18281,7 +18281,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -18290,12 +18290,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>AZO</t>
+          <t>META</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="n">
-        <v>15.17</v>
+        <v>15.09</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -18313,7 +18313,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="K100" t="n">
@@ -18322,21 +18322,21 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>1954</v>
+        <v>3219</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Pat Dorsey - Dorsey Asset Management</t>
+          <t>Yacktman Asset Management</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>META</t>
+          <t>CATO</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="n">
-        <v>15.09</v>
+        <v>15.02</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -18354,7 +18354,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>Consumer Discretionary</t>
         </is>
       </c>
       <c r="K101" t="n">
@@ -18432,10 +18432,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>846.9</v>
+        <v>846.27</v>
       </c>
       <c r="E2" t="n">
-        <v>27.32</v>
+        <v>27.3</v>
       </c>
       <c r="F2" t="n">
         <v>84.81999999999999</v>
@@ -18459,10 +18459,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>223.1</v>
+        <v>225.41</v>
       </c>
       <c r="E3" t="n">
-        <v>13.94</v>
+        <v>14.09</v>
       </c>
       <c r="F3" t="n">
         <v>60.49</v>
@@ -18918,10 +18918,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98.44</v>
+        <v>97.38</v>
       </c>
       <c r="E20" t="n">
-        <v>12.3</v>
+        <v>12.17</v>
       </c>
       <c r="F20" t="n">
         <v>25.76</v>
@@ -19026,10 +19026,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>171.81</v>
+        <v>170.92</v>
       </c>
       <c r="E24" t="n">
-        <v>24.54</v>
+        <v>24.42</v>
       </c>
       <c r="F24" t="n">
         <v>99.58</v>
@@ -19080,13 +19080,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>106</v>
+        <v>105.57</v>
       </c>
       <c r="E26" t="n">
-        <v>15.14</v>
+        <v>15.08</v>
       </c>
       <c r="F26" t="n">
-        <v>26.33</v>
+        <v>25.9</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -19134,13 +19134,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>139.81</v>
+        <v>144.81</v>
       </c>
       <c r="E28" t="n">
-        <v>19.97</v>
+        <v>20.69</v>
       </c>
       <c r="F28" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -19269,10 +19269,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>74.02</v>
+        <v>76.28</v>
       </c>
       <c r="E33" t="n">
-        <v>10.57</v>
+        <v>10.9</v>
       </c>
       <c r="F33" t="n">
         <v>27.96</v>
@@ -19581,7 +19581,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Li Lu - Himalaya Capital Management</t>
+          <t>Nelson Peltz - Trian Fund Management</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -19589,17 +19589,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BAC, BRK.B, GOOGL, GOOG, EWBC</t>
+          <t>JHG, GE, SOLV, WEN, IVZ</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>94.08</v>
+        <v>90.98</v>
       </c>
       <c r="E45" t="n">
-        <v>18.82</v>
+        <v>18.2</v>
       </c>
       <c r="F45" t="n">
-        <v>26.12</v>
+        <v>30.84</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -19608,7 +19608,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Nelson Peltz - Trian Fund Management</t>
+          <t>Mairs &amp; Power Growth Fund</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -19616,17 +19616,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>JHG, GE, SOLV, WEN, IVZ</t>
+          <t>MSFT, NVDA, AMZN, UNH, JPM</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>90.98</v>
+        <v>34.92</v>
       </c>
       <c r="E46" t="n">
-        <v>18.2</v>
+        <v>6.98</v>
       </c>
       <c r="F46" t="n">
-        <v>30.84</v>
+        <v>9.67</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -19635,7 +19635,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Mairs &amp; Power Growth Fund</t>
+          <t>Li Lu - Himalaya Capital Management</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -19643,17 +19643,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MSFT, NVDA, AMZN, UNH, JPM</t>
+          <t>BAC, BRK.B, GOOGL, GOOG, EWBC</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>34.92</v>
+        <v>94.08</v>
       </c>
       <c r="E47" t="n">
-        <v>6.98</v>
+        <v>18.82</v>
       </c>
       <c r="F47" t="n">
-        <v>9.67</v>
+        <v>26.12</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -19689,25 +19689,25 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Chase Coleman - Tiger Global Management</t>
+          <t>Leon Cooperman</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>META, MSFT, SE, GOOGL</t>
+          <t>COOP, ET, APO, VRT, BBDC</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>38.85</v>
+        <v>42.29</v>
       </c>
       <c r="E49" t="n">
-        <v>9.710000000000001</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="F49" t="n">
-        <v>16.18</v>
+        <v>13.58</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -19743,7 +19743,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Yacktman Asset Management</t>
+          <t>Chase Coleman - Tiger Global Management</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -19751,17 +19751,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CNQ, MSFT, AMRK, CATO</t>
+          <t>META, MSFT, SE, GOOGL</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>55.24</v>
+        <v>38.85</v>
       </c>
       <c r="E51" t="n">
-        <v>13.81</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="F51" t="n">
-        <v>21.74</v>
+        <v>16.18</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -19904,7 +19904,7 @@
         <v>54</v>
       </c>
       <c r="E4" t="n">
-        <v>1.82</v>
+        <v>1.8</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -19994,7 +19994,7 @@
         <v>67</v>
       </c>
       <c r="E7" t="n">
-        <v>3.94</v>
+        <v>3.92</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -20024,7 +20024,7 @@
         <v>59</v>
       </c>
       <c r="E8" t="n">
-        <v>3.62</v>
+        <v>3.61</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -20054,7 +20054,7 @@
         <v>48</v>
       </c>
       <c r="E9" t="n">
-        <v>2.1</v>
+        <v>2.12</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -20234,7 +20234,7 @@
         <v>17</v>
       </c>
       <c r="E15" t="n">
-        <v>4.11</v>
+        <v>4.21</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>

</xml_diff>